<commit_message>
add tieumuc vao muchi
</commit_message>
<xml_diff>
--- a/WebApp/wwwroot/template/TemplateImportExpense.xlsx
+++ b/WebApp/wwwroot/template/TemplateImportExpense.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\OnGIT\CreditRequestSystem\WebApp\wwwroot\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t xml:space="preserve">Thông Tin Import </t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>HTV2</t>
+  </si>
+  <si>
+    <t>Tiểu mục</t>
   </si>
 </sst>
 </file>
@@ -474,28 +477,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" style="3" customWidth="1"/>
+    <col min="3" max="4" width="38.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-    </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E1" s="10"/>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
@@ -505,11 +509,14 @@
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -520,7 +527,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
@@ -533,7 +540,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>